<commit_message>
Back to stable version
</commit_message>
<xml_diff>
--- a/temp-peyroll-form/payroll-1.xlsx
+++ b/temp-peyroll-form/payroll-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Congty\thienphumut\test\thienphumut-hr-backend\temp-peyroll-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872EBA1B-383F-4B77-9ABB-12FEDEBF72C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF13D689-6A57-4FDD-938C-C4F97833BFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{81214E9B-BDE1-47CB-8066-A0A8D69825C9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{81214E9B-BDE1-47CB-8066-A0A8D69825C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
@@ -474,59 +474,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="10" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -903,7 +900,7 @@
   <dimension ref="A1:O183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:E6"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -926,78 +923,78 @@
   <sheetData>
     <row r="1" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21"/>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:15" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:15" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="35"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:15" ht="30.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:15" ht="31.3" x14ac:dyDescent="0.35">
       <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="26" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26" t="s">
+      <c r="G5" s="32"/>
+      <c r="H5" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:15" ht="31.3" x14ac:dyDescent="0.35">
       <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="26" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="32"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
         <v>5</v>
@@ -1007,62 +1004,62 @@
       <c r="B7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="26" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="32"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
     </row>
     <row r="8" spans="1:15" ht="31.3" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="26" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="32"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
     </row>
     <row r="9" spans="1:15" ht="30.9" x14ac:dyDescent="0.35">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
     </row>
     <row r="10" spans="1:15" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="39"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="10" t="s">
         <v>5</v>
       </c>
@@ -1075,15 +1072,15 @@
       <c r="I10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
     </row>
     <row r="11" spans="1:15" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9">
         <v>0</v>
@@ -1102,10 +1099,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="61.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="27"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="8"/>
       <c r="E12" s="9">
         <v>0</v>
@@ -1124,10 +1121,10 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10" t="s">
@@ -1142,10 +1139,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9">
         <v>0</v>
@@ -1162,10 +1159,10 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9">
         <v>0</v>
@@ -1182,10 +1179,10 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9">
         <v>0</v>
@@ -1204,10 +1201,10 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="8"/>
       <c r="E17" s="9">
         <v>0</v>
@@ -1226,10 +1223,10 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9">
         <v>0</v>
@@ -1248,10 +1245,10 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9">
         <v>0</v>
@@ -1270,10 +1267,10 @@
       </c>
     </row>
     <row r="20" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9">
         <v>0</v>
@@ -1292,10 +1289,10 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10" t="s">
@@ -1312,10 +1309,10 @@
       </c>
     </row>
     <row r="22" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="12"/>
       <c r="E22" s="9"/>
       <c r="F22" s="10" t="s">
@@ -1332,11 +1329,11 @@
       </c>
     </row>
     <row r="23" spans="2:9" ht="31.3" x14ac:dyDescent="0.35">
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="13">
         <f>+SUM(E10:E21)+SUM(H10:H21)</f>
         <v>0</v>
@@ -1349,10 +1346,10 @@
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="25"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="7" t="s">
         <v>32</v>
       </c>
@@ -1373,8 +1370,8 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="7" t="s">
         <v>34</v>
       </c>
@@ -1395,8 +1392,8 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="7" t="s">
         <v>36</v>
       </c>
@@ -1417,8 +1414,8 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="7" t="s">
         <v>38</v>
       </c>
@@ -1435,11 +1432,11 @@
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="2:9" ht="31.3" x14ac:dyDescent="0.35">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="13">
         <f>+SUM(E24:E27)+SUM(H24:H27)</f>
         <v>40000</v>
@@ -1466,11 +1463,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="2:9" ht="31.3" x14ac:dyDescent="0.75">
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="13">
         <f>+ROUND(E23-E28,0)</f>
         <v>-40000</v>
@@ -1487,56 +1484,56 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
     </row>
     <row r="32" spans="2:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
     </row>
     <row r="33" spans="2:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
     </row>
     <row r="34" spans="2:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
     </row>
     <row r="35" spans="2:9" ht="176.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
     </row>
     <row r="36" spans="2:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="F36" s="17"/>
@@ -1984,12 +1981,16 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:I4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="M7:O10"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B9:I9"/>
     <mergeCell ref="B31:I35"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B11:C11"/>
@@ -2004,16 +2005,12 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="M7:O10"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B1:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>